<commit_message>
Added fix for excel data extraction
</commit_message>
<xml_diff>
--- a/src/test/java/ExternalFiles/TestData.xlsx
+++ b/src/test/java/ExternalFiles/TestData.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
-    <t>TestCase1</t>
-  </si>
-  <si>
     <t>Firstname</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>CheckAddNewEmailbutton</t>
+  </si>
+  <si>
+    <t>CreateContact</t>
   </si>
 </sst>
 </file>
@@ -404,105 +404,105 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>